<commit_message>
update result of fedadagard
</commit_message>
<xml_diff>
--- a/Implement_google_AdaptiveFL/ExperimentRecords.xlsx
+++ b/Implement_google_AdaptiveFL/ExperimentRecords.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\KuihaoFL\Implement_google_AdaptiveFL\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{821DA027-B83F-46BB-AA47-40E9FAE5AA14}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A64B61C-F714-4969-8F41-7FE14BD147E1}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22118" windowHeight="8502" xr2:uid="{0F73F181-28AE-4BA3-A7EA-88CE7E039F5D}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="40">
   <si>
     <t>Aggregation</t>
   </si>
@@ -228,6 +228,22 @@
     <t>發散</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
+  <si>
+    <t>-3</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>-1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>發散?</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>overfit</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
 </sst>
 </file>
 
@@ -236,7 +252,7 @@
   <numFmts count="1">
     <numFmt numFmtId="176" formatCode="0.00_ "/>
   </numFmts>
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -285,6 +301,18 @@
       <family val="3"/>
       <charset val="136"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
   </fonts>
   <fills count="4">
     <fill>
@@ -320,7 +348,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -360,6 +388,15 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="176" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="176" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -367,6 +404,12 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -683,10 +726,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5A9E8C63-6188-4D0F-998D-570A01732085}">
-  <dimension ref="A1:L17"/>
+  <dimension ref="A1:L19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M11" sqref="M11"/>
+      <selection activeCell="D12" sqref="D12:F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.55" x14ac:dyDescent="0.3"/>
@@ -699,7 +742,7 @@
     <col min="12" max="16384" width="8.796875" style="6"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -728,7 +771,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:12" ht="16.149999999999999" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:11" ht="16.149999999999999" x14ac:dyDescent="0.3">
       <c r="B2" s="1" t="s">
         <v>1</v>
       </c>
@@ -755,23 +798,23 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A3" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="B3" s="12" t="s">
+      <c r="B3" s="15" t="s">
         <v>15</v>
       </c>
-      <c r="C3" s="12" t="s">
+      <c r="C3" s="15" t="s">
         <v>12</v>
       </c>
-      <c r="D3" s="15">
+      <c r="D3" s="18">
         <v>-1</v>
       </c>
-      <c r="E3" s="15" t="s">
+      <c r="E3" s="18" t="s">
         <v>20</v>
       </c>
-      <c r="F3" s="15" t="s">
+      <c r="F3" s="18" t="s">
         <v>13</v>
       </c>
       <c r="G3" s="7" t="s">
@@ -787,34 +830,34 @@
         <v>0.44700000000000001</v>
       </c>
     </row>
-    <row r="4" spans="1:12" ht="16.149999999999999" x14ac:dyDescent="0.3">
-      <c r="A4" s="12" t="s">
+    <row r="4" spans="1:11" ht="16.149999999999999" x14ac:dyDescent="0.3">
+      <c r="A4" s="15" t="s">
         <v>11</v>
       </c>
-      <c r="B4" s="12"/>
-      <c r="C4" s="12"/>
-      <c r="D4" s="15"/>
-      <c r="E4" s="15"/>
-      <c r="F4" s="15"/>
-      <c r="G4" s="13" t="s">
+      <c r="B4" s="15"/>
+      <c r="C4" s="15"/>
+      <c r="D4" s="18"/>
+      <c r="E4" s="18"/>
+      <c r="F4" s="18"/>
+      <c r="G4" s="16" t="s">
         <v>30</v>
       </c>
-      <c r="H4" s="14"/>
-      <c r="I4" s="14"/>
-      <c r="J4" s="14"/>
+      <c r="H4" s="17"/>
+      <c r="I4" s="17"/>
+      <c r="J4" s="17"/>
       <c r="K4" s="11" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A5" s="12"/>
-      <c r="B5" s="12"/>
-      <c r="C5" s="12"/>
-      <c r="D5" s="15"/>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A5" s="15"/>
+      <c r="B5" s="15"/>
+      <c r="C5" s="15"/>
+      <c r="D5" s="18"/>
       <c r="E5" s="8">
         <v>0</v>
       </c>
-      <c r="F5" s="15"/>
+      <c r="F5" s="18"/>
       <c r="G5" s="7">
         <v>0.54600000000000004</v>
       </c>
@@ -828,23 +871,23 @@
         <v>0.17</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A6" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="B6" s="12" t="s">
+      <c r="B6" s="15" t="s">
         <v>16</v>
       </c>
-      <c r="C6" s="12" t="s">
+      <c r="C6" s="15" t="s">
         <v>14</v>
       </c>
-      <c r="D6" s="15" t="s">
+      <c r="D6" s="18" t="s">
         <v>22</v>
       </c>
-      <c r="E6" s="15" t="s">
+      <c r="E6" s="18" t="s">
         <v>23</v>
       </c>
-      <c r="F6" s="15" t="s">
+      <c r="F6" s="18" t="s">
         <v>13</v>
       </c>
       <c r="G6" s="7" t="s">
@@ -860,15 +903,15 @@
         <v>0.52400000000000002</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A7" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="B7" s="12"/>
-      <c r="C7" s="12"/>
-      <c r="D7" s="15"/>
-      <c r="E7" s="15"/>
-      <c r="F7" s="15"/>
+      <c r="B7" s="15"/>
+      <c r="C7" s="15"/>
+      <c r="D7" s="18"/>
+      <c r="E7" s="18"/>
+      <c r="F7" s="18"/>
       <c r="G7" s="7">
         <v>0.15540000000000001</v>
       </c>
@@ -882,7 +925,7 @@
         <v>0.1638</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A8" s="4" t="s">
         <v>18</v>
       </c>
@@ -903,7 +946,7 @@
         <v>0.47899999999999998</v>
       </c>
     </row>
-    <row r="9" spans="1:12" ht="16.149999999999999" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:11" ht="16.149999999999999" x14ac:dyDescent="0.3">
       <c r="A9" s="6" t="s">
         <v>11</v>
       </c>
@@ -926,14 +969,14 @@
       <c r="I9" s="7">
         <v>12.646800000000001</v>
       </c>
-      <c r="J9" s="7">
+      <c r="J9" s="19">
         <v>7.8E-2</v>
       </c>
       <c r="K9" s="10" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:11" ht="16.149999999999999" x14ac:dyDescent="0.3">
       <c r="C10" s="2"/>
       <c r="D10" s="8" t="s">
         <v>28</v>
@@ -944,76 +987,109 @@
       <c r="F10" s="8" t="s">
         <v>29</v>
       </c>
-      <c r="J10" s="3"/>
-    </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="G10" s="7">
+        <v>2.1371129999999998</v>
+      </c>
+      <c r="H10" s="7">
+        <v>0.43856000000000001</v>
+      </c>
+      <c r="I10" s="7">
+        <v>30.382121000000001</v>
+      </c>
+      <c r="J10" s="19">
+        <v>4.6879999999999998E-2</v>
+      </c>
+      <c r="K10" s="10" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" s="12" customFormat="1" ht="16.149999999999999" x14ac:dyDescent="0.3">
       <c r="C11" s="2"/>
-      <c r="D11" s="6">
+      <c r="D11" s="14" t="s">
+        <v>37</v>
+      </c>
+      <c r="E11" s="14" t="s">
+        <v>36</v>
+      </c>
+      <c r="F11" s="14" t="s">
+        <v>37</v>
+      </c>
+      <c r="G11" s="13">
+        <v>3.4929999999999999</v>
+      </c>
+      <c r="H11" s="13">
+        <v>0.17643900000000001</v>
+      </c>
+      <c r="I11" s="13">
+        <v>5.3277000000000001</v>
+      </c>
+      <c r="J11" s="19">
+        <v>6.3799999999999996E-2</v>
+      </c>
+      <c r="K11" s="10" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" s="12" customFormat="1" ht="16.149999999999999" x14ac:dyDescent="0.3">
+      <c r="C12" s="2"/>
+      <c r="D12" s="14" t="s">
+        <v>37</v>
+      </c>
+      <c r="E12" s="14" t="s">
+        <v>36</v>
+      </c>
+      <c r="F12" s="14" t="s">
+        <v>36</v>
+      </c>
+      <c r="G12" s="13">
+        <v>0.72512799999999999</v>
+      </c>
+      <c r="H12" s="20">
+        <v>0.79700998999999995</v>
+      </c>
+      <c r="I12" s="13">
+        <v>983.02229999999997</v>
+      </c>
+      <c r="J12" s="19">
+        <v>1.025E-2</v>
+      </c>
+      <c r="K12" s="10" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" ht="16.149999999999999" x14ac:dyDescent="0.3">
+      <c r="C13" s="2"/>
+      <c r="D13" s="6">
         <v>-1</v>
       </c>
-      <c r="E11" s="6">
+      <c r="E13" s="6">
         <v>-4</v>
       </c>
-      <c r="F11" s="6">
+      <c r="F13" s="6">
         <v>-2</v>
       </c>
-    </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A12" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="B12" s="6" t="s">
-        <v>26</v>
-      </c>
-      <c r="C12" s="2"/>
-      <c r="D12" s="8">
-        <f>-3/2</f>
-        <v>-1.5</v>
-      </c>
-      <c r="E12" s="8">
-        <v>0</v>
-      </c>
-      <c r="F12" s="8">
-        <v>-1</v>
-      </c>
-      <c r="J12" s="5">
-        <v>0.52500000000000002</v>
-      </c>
-    </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A13" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="C13" s="2"/>
-      <c r="D13" s="8">
-        <f>-3/2</f>
-        <v>-1.5</v>
-      </c>
-      <c r="E13" s="8">
-        <v>0</v>
-      </c>
-      <c r="F13" s="8">
-        <v>-1</v>
-      </c>
       <c r="G13" s="7">
-        <v>0.33500000000000002</v>
+        <v>3.6149800000000001</v>
       </c>
       <c r="H13" s="7">
-        <v>0.89690000000000003</v>
-      </c>
-      <c r="I13" s="7">
-        <v>6.423</v>
-      </c>
-      <c r="J13" s="3">
-        <v>0.1923</v>
-      </c>
-    </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.3">
+        <v>0.15959999999999999</v>
+      </c>
+      <c r="I13" s="13">
+        <v>232.63688769999999</v>
+      </c>
+      <c r="J13" s="19">
+        <v>9.2999999999999992E-3</v>
+      </c>
+      <c r="K13" s="10" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A14" s="4" t="s">
         <v>18</v>
       </c>
       <c r="B14" s="6" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C14" s="2"/>
       <c r="D14" s="8">
@@ -1027,72 +1103,64 @@
         <v>-1</v>
       </c>
       <c r="J14" s="5">
-        <v>0.52400000000000002</v>
-      </c>
-    </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.3">
+        <v>0.52500000000000002</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A15" s="6" t="s">
         <v>11</v>
       </c>
       <c r="C15" s="2"/>
-      <c r="D15" s="6">
+      <c r="D15" s="8">
+        <f>-3/2</f>
         <v>-1.5</v>
       </c>
-      <c r="E15" s="6">
+      <c r="E15" s="8">
         <v>0</v>
       </c>
-      <c r="F15" s="6">
+      <c r="F15" s="8">
         <v>-1</v>
       </c>
       <c r="G15" s="7">
-        <v>0.32911000000000001</v>
+        <v>0.33500000000000002</v>
       </c>
       <c r="H15" s="7">
-        <v>0.89700000000000002</v>
+        <v>0.89690000000000003</v>
       </c>
       <c r="I15" s="7">
-        <v>5.3682999999999996</v>
+        <v>6.423</v>
       </c>
       <c r="J15" s="3">
-        <v>0.23960000000000001</v>
-      </c>
-      <c r="K15" s="9" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="16" spans="1:12" ht="16.149999999999999" x14ac:dyDescent="0.3">
-      <c r="A16" s="6" t="s">
+        <v>0.1923</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A16" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="B16" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="C16" s="2"/>
+      <c r="D16" s="8">
+        <f>-3/2</f>
+        <v>-1.5</v>
+      </c>
+      <c r="E16" s="8">
+        <v>0</v>
+      </c>
+      <c r="F16" s="8">
+        <v>-1</v>
+      </c>
+      <c r="J16" s="5">
+        <v>0.52400000000000002</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A17" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="D16" s="6">
-        <v>-1.5</v>
-      </c>
-      <c r="E16" s="6">
-        <v>0</v>
-      </c>
-      <c r="F16" s="6">
-        <v>-1</v>
-      </c>
-      <c r="G16" s="7">
-        <v>0.16400000000000001</v>
-      </c>
-      <c r="H16" s="7">
-        <v>0.94840000000000002</v>
-      </c>
-      <c r="I16" s="7">
-        <v>4.7967000000000004</v>
-      </c>
-      <c r="J16" s="3">
-        <v>0.32050000000000001</v>
-      </c>
-      <c r="K16" s="9" t="s">
-        <v>25</v>
-      </c>
-      <c r="L16" s="9" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="17" spans="4:11" ht="16.149999999999999" x14ac:dyDescent="0.3">
+      <c r="C17" s="2"/>
       <c r="D17" s="6">
         <v>-1.5</v>
       </c>
@@ -1103,18 +1171,76 @@
         <v>-1</v>
       </c>
       <c r="G17" s="7">
+        <v>0.32911000000000001</v>
+      </c>
+      <c r="H17" s="7">
+        <v>0.89700000000000002</v>
+      </c>
+      <c r="I17" s="7">
+        <v>5.3682999999999996</v>
+      </c>
+      <c r="J17" s="3">
+        <v>0.23960000000000001</v>
+      </c>
+      <c r="K17" s="9" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12" ht="16.149999999999999" x14ac:dyDescent="0.3">
+      <c r="A18" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="D18" s="6">
+        <v>-1.5</v>
+      </c>
+      <c r="E18" s="6">
+        <v>0</v>
+      </c>
+      <c r="F18" s="6">
+        <v>-1</v>
+      </c>
+      <c r="G18" s="7">
+        <v>0.16400000000000001</v>
+      </c>
+      <c r="H18" s="7">
+        <v>0.94840000000000002</v>
+      </c>
+      <c r="I18" s="7">
+        <v>4.7967000000000004</v>
+      </c>
+      <c r="J18" s="3">
+        <v>0.32050000000000001</v>
+      </c>
+      <c r="K18" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="L18" s="9" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12" ht="16.149999999999999" x14ac:dyDescent="0.3">
+      <c r="D19" s="6">
+        <v>-1.5</v>
+      </c>
+      <c r="E19" s="6">
+        <v>0</v>
+      </c>
+      <c r="F19" s="6">
+        <v>-1</v>
+      </c>
+      <c r="G19" s="7">
         <v>1.6489E-4</v>
       </c>
-      <c r="H17" s="7">
+      <c r="H19" s="7">
         <v>1</v>
       </c>
-      <c r="I17" s="7">
+      <c r="I19" s="7">
         <v>4.0859946799999998</v>
       </c>
-      <c r="J17" s="3">
+      <c r="J19" s="3">
         <v>0.32474999999999998</v>
       </c>
-      <c r="K17" s="9" t="s">
+      <c r="K19" s="9" t="s">
         <v>33</v>
       </c>
     </row>

</xml_diff>